<commit_message>
New tooltips and updated hydrostatic pressure calculator
</commit_message>
<xml_diff>
--- a/assets/resources/version_history.xlsx
+++ b/assets/resources/version_history.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6ff24e4f1aa7cd16/Documents/Deleum/ToolStringEditor/assets/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{A90671B2-A0FF-45E0-93A1-ACAE0189C939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76F0C5C5-164A-458E-B5D2-C4128914194F}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{A90671B2-A0FF-45E0-93A1-ACAE0189C939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54F185ED-0FA7-4702-AD87-11B5E002B534}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="384" yWindow="384" windowWidth="11712" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="720" windowWidth="11712" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
     <t>1.4</t>
   </si>
   <si>
-    <t>Updated tool database. Faster export time. Fixed output of several widgets.</t>
+    <t>Updated tool database. Faster export time. Updated hydrostatic calculation.</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
New logging program app
</commit_message>
<xml_diff>
--- a/assets/resources/version_history.xlsx
+++ b/assets/resources/version_history.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6ff24e4f1aa7cd16/Documents/Deleum/ToolStringEditor/assets/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adammohdtaufik\PycharmProjects\ToolStringEditor\assets\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{A90671B2-A0FF-45E0-93A1-ACAE0189C939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E990086-379B-44F9-9ECF-1A65D0763B9D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB9B027-BA94-4CD1-8A2C-8B00ECE3DC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Version</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>Developed PCE Stack Up Editor. Updated PCE and DHT databases.</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>New calculations available in calculator</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>Introduced Logging Planner app</t>
   </si>
 </sst>
 </file>
@@ -139,13 +151,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B31BF61C-4FAC-4A44-A80D-2526246C1DE3}" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0">
-  <autoFilter ref="A1:D7" xr:uid="{B31BF61C-4FAC-4A44-A80D-2526246C1DE3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B31BF61C-4FAC-4A44-A80D-2526246C1DE3}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0">
+  <autoFilter ref="A1:D9" xr:uid="{B31BF61C-4FAC-4A44-A80D-2526246C1DE3}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D2B7D2EA-AA20-41EA-919D-97B6DF5E413E}" name="Version" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{A4773B05-95E1-4F28-A1F8-54BC68CE783E}" name="Updates"/>
@@ -419,21 +427,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,87 +455,115 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2">
+        <v>46052</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2">
+        <v>46045</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D4" s="2">
         <v>45939</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
         <v>45902</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2">
         <v>45850</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2">
         <v>45788</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2">
         <v>45765</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2">
         <v>45736</v>
       </c>
     </row>

</xml_diff>